<commit_message>
fully tested scheduler with partitioner
</commit_message>
<xml_diff>
--- a/autocomm_v2/commute.xlsx
+++ b/autocomm_v2/commute.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rushi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E4AF4-3663-4C10-9ED4-0F67B5AE9F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93E186-16CC-4776-A723-3ED8AA2743FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6186EC3D-C133-4060-B20B-059475437E28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6186EC3D-C133-4060-B20B-059475437E28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="63">
   <si>
     <t>lgtype</t>
   </si>
@@ -931,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172847D3-4CC1-45D0-81CB-F341FE3C4940}">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,6 +3107,21 @@
         <v>62</v>
       </c>
     </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D129" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129" s="33"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>